<commit_message>
Fixed a typo in reference files and corrected data type for two fields.
</commit_message>
<xml_diff>
--- a/static/fields/drugshortages_reference.xlsx
+++ b/static/fields/drugshortages_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10315"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/violet.wren/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B48100-B05A-9F49-BF4E-E89C0BC9DFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE719C0-8E88-5246-A822-F802064EB670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="760" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>Presntation shortage status</t>
-  </si>
-  <si>
     <t>update_date</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>The list of active ingredients of a drug product.</t>
+  </si>
+  <si>
+    <t>Presentation shortage status</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1134,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1309,7 @@
         <v>67</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>66</v>
@@ -1331,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>68</v>
@@ -1345,51 +1345,51 @@
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1400,7 +1400,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>14</v>
@@ -1414,7 +1414,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>18</v>
@@ -1428,7 +1428,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>26</v>
@@ -1442,7 +1442,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>28</v>
@@ -1456,7 +1456,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>29</v>
@@ -1467,13 +1467,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1484,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>23</v>
@@ -1498,7 +1498,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>32</v>
@@ -1512,7 +1512,7 @@
         <v>33</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>40</v>
@@ -1526,7 +1526,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>41</v>
@@ -1540,7 +1540,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>42</v>
@@ -1554,7 +1554,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>8</v>
@@ -1568,7 +1568,7 @@
         <v>11</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>12</v>
@@ -1582,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>20</v>
@@ -1596,7 +1596,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>43</v>
@@ -1610,7 +1610,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>10</v>
@@ -1624,7 +1624,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>44</v>
@@ -1635,13 +1635,13 @@
         <v>24</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1652,7 +1652,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>45</v>
@@ -1666,7 +1666,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>46</v>
@@ -1676,7 +1676,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="57" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="56" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>